<commit_message>
Fix the excel date/time cell translation
</commit_message>
<xml_diff>
--- a/tests/1table.xlsx
+++ b/tests/1table.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verge\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\verge\GIT\excel2csv\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Creation date</t>
   </si>
@@ -45,12 +45,36 @@
   </si>
   <si>
     <t>Weight(g)</t>
+  </si>
+  <si>
+    <t>monitor</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>0/0/0</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>1/3/1689 8:34:00 AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,9 +104,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,15 +427,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -424,8 +454,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>36526</v>
+      <c r="A2" s="2">
+        <v>0.57291666666666663</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -439,8 +469,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>38352</v>
+      <c r="A3" s="3">
+        <v>0.99722222222222223</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -455,7 +485,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>37848</v>
+        <v>37623</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -468,7 +498,78 @@
         <v>4200</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>7.8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>38412.524259259262</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>9.4</v>
+      </c>
+      <c r="D8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>-1.3</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>